<commit_message>
final all files batch module submit
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData/AddBatchModule.xlsx
+++ b/src/test/resources/ExcelTestData/AddBatchModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subas\EclipseLMSPractice\Team15_SeleniumTribe_LMSUIHackathon_Apr24\src\test\resources\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10641E4-A809-4854-B8A8-840B3C7D7A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26BC216-2D97-41AB-A219-3418650827DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{935A3F96-FF7B-4344-8DBC-4AB257648386}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>S.no</t>
   </si>
@@ -65,9 +65,6 @@
     <t>InvalidValues</t>
   </si>
   <si>
-    <t>!@3</t>
-  </si>
-  <si>
     <t>batchField</t>
   </si>
   <si>
@@ -126,13 +123,28 @@
   </si>
   <si>
     <t>Updated Description</t>
+  </si>
+  <si>
+    <t>!@3*&amp;Invalid</t>
+  </si>
+  <si>
+    <t>This field should start with an alphabet and min 2 character.</t>
+  </si>
+  <si>
+    <t>errormsg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>Invalid without optionaldesc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +172,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -194,6 +213,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -529,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90273CE1-256D-4D00-BB28-CAB5D5AD9851}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,9 +570,10 @@
     <col min="8" max="8" width="34.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="33.5546875" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,10 +587,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
@@ -573,13 +599,16 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -596,22 +625,25 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -624,52 +656,64 @@
       <c r="D3">
         <v>3</v>
       </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
       <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
-        <v>21</v>
+      <c r="J4" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H4" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>